<commit_message>
handle synonyms with no accepted name
</commit_message>
<xml_diff>
--- a/input/reviewed_duplicates.xlsx
+++ b/input/reviewed_duplicates.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3DEF745-6ACD-4AB8-9F4B-422DCE82E880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{C3DEF745-6ACD-4AB8-9F4B-422DCE82E880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{048E3756-0EB0-4B3E-BCE4-72F982562D9D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lewis_duplicates" sheetId="1" r:id="rId1"/>
@@ -298,9 +298,6 @@
     <t>Acediopsylla Ewing, 1940; Cediopsylla Jordan, 1925</t>
   </si>
   <si>
-    <t>Lewis2404</t>
-  </si>
-  <si>
     <t>Acediopsylla Ewing, 1940</t>
   </si>
   <si>
@@ -320,12 +317,15 @@
   </si>
   <si>
     <t>Jordan, 1925</t>
+  </si>
+  <si>
+    <t>Lewis12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1159,15 +1159,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AN12" sqref="AN12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="18" max="18" width="34.36328125" customWidth="1"/>
     <col min="40" max="40" width="33.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1319,7 +1320,7 @@
         <v>46</v>
       </c>
       <c r="I2">
-        <v>2998</v>
+        <v>2790</v>
       </c>
       <c r="J2" t="s">
         <v>43</v>
@@ -1328,28 +1329,28 @@
         <v>43</v>
       </c>
       <c r="L2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>93</v>
-      </c>
-      <c r="S2" t="s">
-        <v>94</v>
       </c>
       <c r="T2" t="s">
         <v>43</v>
@@ -1388,13 +1389,13 @@
         <v>43</v>
       </c>
       <c r="AF2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH2" t="s">
         <v>95</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>96</v>
       </c>
       <c r="AI2" t="s">
         <v>43</v>
@@ -1423,7 +1424,7 @@
         <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>90</v>
@@ -1441,7 +1442,7 @@
         <v>46</v>
       </c>
       <c r="I3">
-        <v>3232</v>
+        <v>3171</v>
       </c>
       <c r="J3" t="s">
         <v>43</v>
@@ -1450,7 +1451,7 @@
         <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="M3" t="s">
         <v>43</v>
@@ -1468,10 +1469,10 @@
         <v>43</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T3" t="s">
         <v>43</v>
@@ -1510,13 +1511,13 @@
         <v>43</v>
       </c>
       <c r="AF3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AG3" t="s">
         <v>43</v>
       </c>
       <c r="AH3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AI3" t="s">
         <v>43</v>
@@ -1534,7 +1535,7 @@
         <v>43</v>
       </c>
       <c r="AN3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.35">
@@ -1563,7 +1564,7 @@
         <v>46</v>
       </c>
       <c r="I4">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="J4" t="s">
         <v>43</v>
@@ -1685,7 +1686,7 @@
         <v>46</v>
       </c>
       <c r="I5">
-        <v>1251</v>
+        <v>319</v>
       </c>
       <c r="J5" t="s">
         <v>43</v>
@@ -1807,7 +1808,7 @@
         <v>46</v>
       </c>
       <c r="I6">
-        <v>2333</v>
+        <v>367</v>
       </c>
       <c r="J6" t="s">
         <v>43</v>
@@ -1929,7 +1930,7 @@
         <v>46</v>
       </c>
       <c r="I7">
-        <v>2532</v>
+        <v>399</v>
       </c>
       <c r="J7" t="s">
         <v>43</v>
@@ -2051,7 +2052,7 @@
         <v>46</v>
       </c>
       <c r="I8">
-        <v>2709</v>
+        <v>417</v>
       </c>
       <c r="J8" t="s">
         <v>43</v>
@@ -2148,8 +2149,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN62">
-    <sortCondition ref="AN2:AN62"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN8">
+    <sortCondition ref="AN2:AN8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>